<commit_message>
Few more spreadsheet tweaks, Marksman adjustments
</commit_message>
<xml_diff>
--- a/Long War Divided/Ability Loc.xlsx
+++ b/Long War Divided/Ability Loc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teddy\Desktop\XCOM 2 Mods\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Teddy\Documents\Firaxis ModBuddy\XCOM\Long War Divided\Long War Divided\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>TemplateName</t>
   </si>
@@ -212,12 +212,27 @@
 Use # to separate elements in Promotion Popup that you want separated by bullets.
 The Substitutions box is for shorthand, so you don't have to type out &lt;Ability:Weapon/&gt; all the time. I dunno, I'm lazy. There's plenty of space for you to put your own in.</t>
   </si>
+  <si>
+    <t>Made by:</t>
+  </si>
+  <si>
+    <t>Teddy McCormick</t>
+  </si>
+  <si>
+    <t>DaTedinator@gmail.com</t>
+  </si>
+  <si>
+    <t>/u/DaTedinator</t>
+  </si>
+  <si>
+    <t>Reddit is more likely to get a quick response than email, but whatever works.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,8 +298,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,8 +362,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -829,17 +858,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -913,15 +1030,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -969,11 +1077,68 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -992,18 +1157,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1018,13 +1171,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D34" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D34" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A2:D34"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Ability Name"/>
-    <tableColumn id="2" name="Ability Description" dataDxfId="4"/>
-    <tableColumn id="3" name="Promotion Popup" dataDxfId="3"/>
-    <tableColumn id="4" name="Miss Message" dataDxfId="2"/>
+    <tableColumn id="2" name="Ability Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Promotion Popup" dataDxfId="1"/>
+    <tableColumn id="4" name="Miss Message" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1329,7 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1340,16 +1495,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="38" t="str">
+      <c r="D1" s="34" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(10),TRUE,Sheet3!A2:A34)</f>
         <v xml:space="preserve">[LWD_AntiMaterielRounds X2AbilityTemplate]
 LocFriendlyName="Anti-Materiel Rounds"
@@ -1431,431 +1586,458 @@
 LocPromotionPopupText="&lt;Bullet/&gt;You always carry a shaped charge into battle, and the radius of your shaped charges is increased.&lt;br/&gt;"
 </v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="35"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="36"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="44"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="48"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="44"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="47"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="26"/>
+      <c r="E12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="11"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="15"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="19"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="21"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="11"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="15"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
     </row>
     <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
     </row>
     <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
     </row>
-    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" t="s">
-        <v>56</v>
-      </c>
+    <row r="22" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
     </row>
     <row r="25" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
       <c r="E25" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
       <c r="E26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
       <c r="E27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
       <c r="E28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
       <c r="E29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
       <c r="E30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
       <c r="E31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
       <c r="E32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
       <c r="E33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
       <c r="E34" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="E22:I22"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="E2:I9"/>
     <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E19:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1964,7 +2146,7 @@
         <v>Anti-Materiel Rounds</v>
       </c>
       <c r="R2" t="str">
-        <f>Q2</f>
+        <f t="shared" ref="R2:R35" si="0">Q2</f>
         <v>Anti-Materiel Rounds</v>
       </c>
       <c r="S2" t="str">
@@ -2022,7 +2204,7 @@
         <v>Gallop</v>
       </c>
       <c r="R3" t="str">
-        <f>Q3</f>
+        <f t="shared" si="0"/>
         <v>Gallop</v>
       </c>
       <c r="S3" t="str">
@@ -2080,7 +2262,7 @@
         <v>Fully Stocked</v>
       </c>
       <c r="R4" t="str">
-        <f>Q4</f>
+        <f t="shared" si="0"/>
         <v>Fully Stocked</v>
       </c>
       <c r="S4" t="str">
@@ -2138,7 +2320,7 @@
         <v>Hands and Feet</v>
       </c>
       <c r="R5" t="str">
-        <f>Q5</f>
+        <f t="shared" si="0"/>
         <v>Hands and Feet</v>
       </c>
       <c r="S5" t="str">
@@ -2196,7 +2378,7 @@
         <v>Artificial Intelligence</v>
       </c>
       <c r="R6" t="str">
-        <f>Q6</f>
+        <f t="shared" si="0"/>
         <v>Artificial Intelligence</v>
       </c>
       <c r="S6" t="str">
@@ -2254,7 +2436,7 @@
         <v>Self-Aware</v>
       </c>
       <c r="R7" t="str">
-        <f>Q7</f>
+        <f t="shared" si="0"/>
         <v>Self-Aware</v>
       </c>
       <c r="S7" t="str">
@@ -2312,7 +2494,7 @@
         <v>Smartlink Protocol</v>
       </c>
       <c r="R8" t="str">
-        <f>Q8</f>
+        <f t="shared" si="0"/>
         <v>Smartlink Protocol</v>
       </c>
       <c r="S8" t="str">
@@ -2370,7 +2552,7 @@
         <v>Jab</v>
       </c>
       <c r="R9" t="str">
-        <f>Q9</f>
+        <f t="shared" si="0"/>
         <v>Jab</v>
       </c>
       <c r="S9" t="str">
@@ -2428,7 +2610,7 @@
         <v>Where It Hurts</v>
       </c>
       <c r="R10" t="str">
-        <f>Q10</f>
+        <f t="shared" si="0"/>
         <v>Where It Hurts</v>
       </c>
       <c r="S10" t="str">
@@ -2486,7 +2668,7 @@
         <v>Tight Choke</v>
       </c>
       <c r="R11" t="str">
-        <f>Q11</f>
+        <f t="shared" si="0"/>
         <v>Tight Choke</v>
       </c>
       <c r="S11" t="str">
@@ -2544,7 +2726,7 @@
         <v>Whites of Their Eyes</v>
       </c>
       <c r="R12" t="str">
-        <f>Q12</f>
+        <f t="shared" si="0"/>
         <v>Whites of Their Eyes</v>
       </c>
       <c r="S12" t="str">
@@ -2602,7 +2784,7 @@
         <v>Cattle Prod</v>
       </c>
       <c r="R13" t="str">
-        <f>Q13</f>
+        <f t="shared" si="0"/>
         <v>Cattle Prod</v>
       </c>
       <c r="S13" t="str">
@@ -2660,7 +2842,7 @@
         <v>Dynamite</v>
       </c>
       <c r="R14" t="str">
-        <f>Q14</f>
+        <f t="shared" si="0"/>
         <v>Dynamite</v>
       </c>
       <c r="S14" t="str">
@@ -2718,7 +2900,7 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <f>Q15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S15">
@@ -2776,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="R16">
-        <f>Q16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S16">
@@ -2834,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <f>Q17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S17">
@@ -2892,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <f>Q18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S18">
@@ -2950,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="R19">
-        <f>Q19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S19">
@@ -3008,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="R20">
-        <f>Q20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S20">
@@ -3066,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <f>Q21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S21">
@@ -3124,7 +3306,7 @@
         <v>0</v>
       </c>
       <c r="R22">
-        <f>Q22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S22">
@@ -3182,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="R23">
-        <f>Q23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S23">
@@ -3240,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <f>Q24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S24">
@@ -3298,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <f>Q25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S25">
@@ -3356,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <f>Q26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S26">
@@ -3414,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="R27">
-        <f>Q27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S27">
@@ -3472,7 +3654,7 @@
         <v>0</v>
       </c>
       <c r="R28">
-        <f>Q28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S28">
@@ -3530,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="R29">
-        <f>Q29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S29">
@@ -3588,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="R30">
-        <f>Q30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S30">
@@ -3646,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="R31">
-        <f>Q31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S31">
@@ -3704,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="R32">
-        <f>Q32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S32">
@@ -3762,7 +3944,7 @@
         <v>0</v>
       </c>
       <c r="R33">
-        <f>Q33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S33">
@@ -3820,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="R34">
-        <f>Q34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S34">
@@ -3850,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="R35">
-        <f>Q35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S35">
@@ -12488,20 +12670,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>